<commit_message>
changes to Security and WCF
</commit_message>
<xml_diff>
--- a/Security.xlsx
+++ b/Security.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Security Attacks" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>CSRF</t>
   </si>
@@ -98,6 +98,12 @@
       </rPr>
       <t>"</t>
     </r>
+  </si>
+  <si>
+    <t>Denial of service attack</t>
+  </si>
+  <si>
+    <t>DOS</t>
   </si>
 </sst>
 </file>
@@ -455,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,6 +480,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -483,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>